<commit_message>
Updated E2E script for Login and Register
</commit_message>
<xml_diff>
--- a/SauceDemoData.xlsx
+++ b/SauceDemoData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vigneshelumalai/Downloads/wep-e2e-automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CF0B5D-2D41-3B4C-AA82-9EC44DAC1EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329258A5-E6A4-894E-98FC-4EB43E6024ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page Content" sheetId="1" r:id="rId1"/>
-    <sheet name="Form Input" sheetId="3" r:id="rId2"/>
+    <sheet name="Login Functionality" sheetId="3" r:id="rId2"/>
     <sheet name="Login Page Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Test Case number</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>Account Deleted</t>
+  </si>
+  <si>
+    <t>User Name Mail</t>
+  </si>
+  <si>
+    <t>test12312122@gmail.com</t>
+  </si>
+  <si>
+    <t>User password</t>
+  </si>
+  <si>
+    <t>Test@12345</t>
   </si>
 </sst>
 </file>
@@ -512,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -718,10 +730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEE54E4-3E05-AD42-9B2B-4869243936CF}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,78 +752,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>600001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>9876543210</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>